<commit_message>
Add bank statement & OCR integrations
Rename app title to "BC ACCOUNT" and add environment variables for bank statement and OCR services (VITE_APP_BANK_STATEMENT_API, VITE_APP_API_OCR). Introduce API clients for bank statements and OCR, plus new accounting UI components and dialogs (AI model selection, OCR result/test, statement config, statement journal/transaction tables, task/image selection) and a JournalFromStatement page. Update many Vue views/layouts/services and firebase hosting/cache to support the new features and integrations. Also include minor updates to package.json, README and other components to accommodate these additions.
</commit_message>
<xml_diff>
--- a/public/demo/file/template_creditors.xlsx
+++ b/public/demo/file/template_creditors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\NONG\DEDE Account\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palm My\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A192A5FD-E6DE-43E0-A42D-719A80849A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FA2A60-A989-4807-8491-CB859A4E4E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="10020" windowWidth="28800" windowHeight="15210" xr2:uid="{D916F5DB-F259-4982-8027-891203CEA8BF}"/>
+    <workbookView xWindow="19090" yWindow="-3710" windowWidth="38620" windowHeight="21100" xr2:uid="{D916F5DB-F259-4982-8027-891203CEA8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,8 +59,8 @@
             <charset val="222"/>
           </rPr>
           <t xml:space="preserve">
-0 = บุคคลธรรมดา
-1 = นิติบุคคล</t>
+1 = บุคคลธรรมดา
+2 = นิติบุคคล</t>
         </r>
       </text>
     </comment>
@@ -84,8 +84,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-0 = สำนักงานใหญ่
-1 = สาขา</t>
+1 = สำนักงานใหญ่
+2 = สาขา</t>
         </r>
       </text>
     </comment>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>รหัสเจ้าหนี้*</t>
   </si>
@@ -153,20 +153,44 @@
     <t>0107567000414</t>
   </si>
   <si>
-    <t>00159</t>
-  </si>
-  <si>
     <t>141/469 หมู่ 7 บ้านศรีบุญเรือง</t>
   </si>
   <si>
     <t>099-9999999</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>AR0002</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>บริษัท ซีพี ออล</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>00001</t>
+  </si>
+  <si>
+    <t>0107567000515</t>
+  </si>
+  <si>
+    <t>515/945 หมู่ 2 บ้านศรีไชย</t>
+  </si>
+  <si>
+    <t>099-1111111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +244,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -255,12 +286,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -279,9 +310,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -319,7 +350,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -425,7 +456,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -567,7 +598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -578,7 +609,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -652,8 +683,8 @@
       <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7">
-        <v>1</v>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>18</v>
@@ -662,26 +693,43 @@
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>